<commit_message>
EPBDS-6361 In the case (Integer) / (Integer) it's expected the real value, not rounded till Integer, for instance 2/3 = 0.6666(6), not 0
</commit_message>
<xml_diff>
--- a/Util/openl-maven-plugin/it/openl-tests-failure/src/main/openl/rules/RulesWithError.xlsx
+++ b/Util/openl-maven-plugin/it/openl-tests-failure/src/main/openl/rules/RulesWithError.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\Util\openl-maven-plugin\it\openl-tests-failure\src\main\openl\rules\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
   </bookViews>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>Greeting</t>
   </si>
@@ -80,12 +85,15 @@
   </si>
   <si>
     <t>="" + hour / 0</t>
+  </si>
+  <si>
+    <t>Infinity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0_ ;_-[$$-409]* \-#,##0\ ;_-[$$-409]* &quot;-&quot;_ ;_-@_ "/>
   </numFmts>
@@ -297,7 +305,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -305,14 +313,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -350,9 +361,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -385,9 +396,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -420,9 +448,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -599,7 +644,7 @@
   <dimension ref="B2:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16:G16"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,7 +712,7 @@
         <v>25</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>